<commit_message>
add a few words about Parallels.Invoke to report
</commit_message>
<xml_diff>
--- a/Reports/ПИ-13-4_Потемкин_ИЗ1.xlsx
+++ b/Reports/ПИ-13-4_Потемкин_ИЗ1.xlsx
@@ -707,6 +707,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -952,6 +953,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -29988,7 +29990,7 @@
       <xdr:row>43</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="10214463" cy="1125693"/>
+    <xdr:ext cx="10492616" cy="1470146"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -29997,7 +29999,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="863600" y="9067800"/>
-          <a:ext cx="10214463" cy="1125693"/>
+          <a:ext cx="10492616" cy="1470146"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -30094,10 +30096,46 @@
         <a:p>
           <a:r>
             <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
-            <a:t>подверджены паралелизации в итоге не дают такого же прироста в производительности как в случае не симдовских матриц.</a:t>
+            <a:t>подверджены паралелизации в итоге не дают такого же прироста в производительности как в случае не симдовских матриц. </a:t>
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100"/>
+            <a:t>Что касается двух способов распаралеливания алгоритма Штрассена, то видно, что</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t> вариант с использование </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>async </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t>и паралелизации на последним шаге обычного метода </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t>перемножения матриц дает результат хуже. Это связано с тем, что </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Parallels.Invoke </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t>сам разбивает на пачки методов, которые должны быть в разных потоках и сам решает </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t>какой наиболее эффективный способ их запуска.</a:t>
+          </a:r>
           <a:endParaRPr lang="ru-RU" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -32296,8 +32334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
some changes in report
</commit_message>
<xml_diff>
--- a/Reports/ПИ-13-4_Потемкин_ИЗ1.xlsx
+++ b/Reports/ПИ-13-4_Потемкин_ИЗ1.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
-  <workbookPr showInkAnnotation="0" hidePivotFieldList="1"/>
+  <workbookPr showInkAnnotation="0" hidePivotFieldList="1" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostemkin/Documents/Personal/PrP/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24840" windowHeight="15540" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24840" windowHeight="15540" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Theory approximate" sheetId="2" state="hidden" r:id="rId1"/>
@@ -226,7 +226,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,6 +290,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -40837,7 +40843,7 @@
       <xdr:row>135</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="10492616" cy="1470146"/>
+    <xdr:ext cx="13187393" cy="1470146"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -40846,7 +40852,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="825500" y="27800300"/>
-          <a:ext cx="10492616" cy="1470146"/>
+          <a:ext cx="13187393" cy="1470146"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -40893,7 +40899,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
-            <a:t>. Также из полученных результов видно, что распаралеливание обычной</a:t>
+            <a:t>. Из полученных результов видно, что распаралеливание обычной</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -40907,7 +40913,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
-            <a:t>, что еще раз </a:t>
+            <a:t>(если брать использование на больших матрицах), что еще раз </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -40975,7 +40981,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
-            <a:t>сам разбивает на пачки методов, которые должны быть в разных потоках и сам решает </a:t>
+            <a:t>сам разбивает на пачки передаваемые методы, которые должны быть в разных потоках и сам решает </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -43633,8 +43639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="H43" sqref="B4:H43"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G151" sqref="G151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -44609,6 +44615,7 @@
     <mergeCell ref="B29:H29"/>
     <mergeCell ref="B37:H37"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -44619,7 +44626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C7:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView topLeftCell="B88" workbookViewId="0">
       <selection activeCell="C43" sqref="C43:I46"/>
     </sheetView>
   </sheetViews>

</xml_diff>